<commit_message>
Update Test case: Shift test case arrange according to new temaplate sequence
</commit_message>
<xml_diff>
--- a/System 6 Renovation Working Files/Test Files/Raw Data (3).xlsx
+++ b/System 6 Renovation Working Files/Test Files/Raw Data (3).xlsx
@@ -5831,35 +5831,8 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -5880,6 +5853,33 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="44" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="44" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="44" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -6230,8 +6230,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:IG1186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FD1" workbookViewId="0">
-      <selection activeCell="FH6" sqref="FH6"/>
+    <sheetView tabSelected="1" topLeftCell="FL1" workbookViewId="0">
+      <selection activeCell="FM12" sqref="FM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6242,7 +6242,7 @@
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -6254,7 +6254,7 @@
     <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15.5703125" customWidth="1"/>
     <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1"/>
@@ -6275,7 +6275,7 @@
     <col min="43" max="43" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="23" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="19.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="19.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -6333,7 +6333,7 @@
     <col min="109" max="109" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="10.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="115" max="115" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="116" max="119" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -6358,7 +6358,7 @@
     <col min="138" max="138" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="139" max="139" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="140" max="140" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="141" max="141" width="9.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="9.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="143" max="143" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="144" max="144" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="145" max="148" width="13.5703125" bestFit="1" customWidth="1"/>
@@ -6378,16 +6378,16 @@
     <col min="162" max="162" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="163" max="163" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="164" max="164" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="12.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="27" bestFit="1" customWidth="1"/>
-    <col min="171" max="171" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="22" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="23" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="27" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="22" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="23" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="23.28515625" customWidth="1"/>
+    <col min="170" max="170" width="12.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="171" max="171" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="175" max="177" width="13.5703125" hidden="1" customWidth="1"/>
     <col min="178" max="178" width="11.140625" hidden="1" customWidth="1"/>
     <col min="179" max="179" width="4.28515625" hidden="1" customWidth="1"/>
@@ -6416,361 +6416,361 @@
     <col min="202" max="202" width="23" hidden="1" customWidth="1"/>
     <col min="203" max="203" width="26.28515625" hidden="1" customWidth="1"/>
     <col min="204" max="241" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="242" max="256" width="9.140625" customWidth="1"/>
+    <col min="242" max="251" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:241" x14ac:dyDescent="0.2">
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="11" t="s">
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1" s="25"/>
+      <c r="AM1" s="25"/>
+      <c r="AN1" s="25"/>
+      <c r="AO1" s="25"/>
+      <c r="AP1" s="25"/>
+      <c r="AQ1" s="25"/>
+      <c r="AR1" s="25"/>
+      <c r="AS1" s="25"/>
+      <c r="AT1" s="25"/>
+      <c r="AU1" s="25"/>
+      <c r="AV1" s="25"/>
+      <c r="AW1" s="25"/>
+      <c r="AX1" s="26"/>
+      <c r="AY1" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
-      <c r="BO1" s="12"/>
-      <c r="BP1" s="12"/>
-      <c r="BQ1" s="12"/>
-      <c r="BR1" s="12"/>
-      <c r="BS1" s="12"/>
-      <c r="BT1" s="12"/>
-      <c r="BU1" s="12"/>
-      <c r="BV1" s="12"/>
-      <c r="BW1" s="12"/>
-      <c r="BX1" s="12"/>
-      <c r="BY1" s="12"/>
-      <c r="BZ1" s="13"/>
-      <c r="CA1" s="11" t="s">
+      <c r="AZ1" s="25"/>
+      <c r="BA1" s="25"/>
+      <c r="BB1" s="25"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="25"/>
+      <c r="BE1" s="25"/>
+      <c r="BF1" s="25"/>
+      <c r="BG1" s="25"/>
+      <c r="BH1" s="25"/>
+      <c r="BI1" s="25"/>
+      <c r="BJ1" s="25"/>
+      <c r="BK1" s="25"/>
+      <c r="BL1" s="25"/>
+      <c r="BM1" s="25"/>
+      <c r="BN1" s="25"/>
+      <c r="BO1" s="25"/>
+      <c r="BP1" s="25"/>
+      <c r="BQ1" s="25"/>
+      <c r="BR1" s="25"/>
+      <c r="BS1" s="25"/>
+      <c r="BT1" s="25"/>
+      <c r="BU1" s="25"/>
+      <c r="BV1" s="25"/>
+      <c r="BW1" s="25"/>
+      <c r="BX1" s="25"/>
+      <c r="BY1" s="25"/>
+      <c r="BZ1" s="26"/>
+      <c r="CA1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="CB1" s="12"/>
-      <c r="CC1" s="12"/>
-      <c r="CD1" s="12"/>
-      <c r="CE1" s="12"/>
-      <c r="CF1" s="12"/>
-      <c r="CG1" s="12"/>
-      <c r="CH1" s="12"/>
-      <c r="CI1" s="12"/>
-      <c r="CJ1" s="12"/>
-      <c r="CK1" s="12"/>
-      <c r="CL1" s="12"/>
-      <c r="CM1" s="12"/>
-      <c r="CN1" s="12"/>
-      <c r="CO1" s="12"/>
-      <c r="CP1" s="12"/>
-      <c r="CQ1" s="12"/>
-      <c r="CR1" s="12"/>
-      <c r="CS1" s="12"/>
-      <c r="CT1" s="12"/>
-      <c r="CU1" s="12"/>
-      <c r="CV1" s="12"/>
-      <c r="CW1" s="12"/>
-      <c r="CX1" s="12"/>
-      <c r="CY1" s="12"/>
-      <c r="CZ1" s="12"/>
-      <c r="DA1" s="12"/>
-      <c r="DB1" s="13"/>
-      <c r="DC1" s="11" t="s">
+      <c r="CB1" s="25"/>
+      <c r="CC1" s="25"/>
+      <c r="CD1" s="25"/>
+      <c r="CE1" s="25"/>
+      <c r="CF1" s="25"/>
+      <c r="CG1" s="25"/>
+      <c r="CH1" s="25"/>
+      <c r="CI1" s="25"/>
+      <c r="CJ1" s="25"/>
+      <c r="CK1" s="25"/>
+      <c r="CL1" s="25"/>
+      <c r="CM1" s="25"/>
+      <c r="CN1" s="25"/>
+      <c r="CO1" s="25"/>
+      <c r="CP1" s="25"/>
+      <c r="CQ1" s="25"/>
+      <c r="CR1" s="25"/>
+      <c r="CS1" s="25"/>
+      <c r="CT1" s="25"/>
+      <c r="CU1" s="25"/>
+      <c r="CV1" s="25"/>
+      <c r="CW1" s="25"/>
+      <c r="CX1" s="25"/>
+      <c r="CY1" s="25"/>
+      <c r="CZ1" s="25"/>
+      <c r="DA1" s="25"/>
+      <c r="DB1" s="26"/>
+      <c r="DC1" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="DD1" s="12"/>
-      <c r="DE1" s="12"/>
-      <c r="DF1" s="12"/>
-      <c r="DG1" s="12"/>
-      <c r="DH1" s="12"/>
-      <c r="DI1" s="12"/>
-      <c r="DJ1" s="12"/>
-      <c r="DK1" s="12"/>
-      <c r="DL1" s="12"/>
-      <c r="DM1" s="12"/>
-      <c r="DN1" s="12"/>
-      <c r="DO1" s="12"/>
-      <c r="DP1" s="12"/>
-      <c r="DQ1" s="12"/>
-      <c r="DR1" s="12"/>
-      <c r="DS1" s="12"/>
-      <c r="DT1" s="12"/>
-      <c r="DU1" s="12"/>
-      <c r="DV1" s="12"/>
-      <c r="DW1" s="12"/>
-      <c r="DX1" s="12"/>
-      <c r="DY1" s="12"/>
-      <c r="DZ1" s="12"/>
-      <c r="EA1" s="12"/>
-      <c r="EB1" s="12"/>
-      <c r="EC1" s="12"/>
-      <c r="ED1" s="12"/>
-      <c r="EE1" s="13"/>
-      <c r="EF1" s="11" t="s">
+      <c r="DD1" s="25"/>
+      <c r="DE1" s="25"/>
+      <c r="DF1" s="25"/>
+      <c r="DG1" s="25"/>
+      <c r="DH1" s="25"/>
+      <c r="DI1" s="25"/>
+      <c r="DJ1" s="25"/>
+      <c r="DK1" s="25"/>
+      <c r="DL1" s="25"/>
+      <c r="DM1" s="25"/>
+      <c r="DN1" s="25"/>
+      <c r="DO1" s="25"/>
+      <c r="DP1" s="25"/>
+      <c r="DQ1" s="25"/>
+      <c r="DR1" s="25"/>
+      <c r="DS1" s="25"/>
+      <c r="DT1" s="25"/>
+      <c r="DU1" s="25"/>
+      <c r="DV1" s="25"/>
+      <c r="DW1" s="25"/>
+      <c r="DX1" s="25"/>
+      <c r="DY1" s="25"/>
+      <c r="DZ1" s="25"/>
+      <c r="EA1" s="25"/>
+      <c r="EB1" s="25"/>
+      <c r="EC1" s="25"/>
+      <c r="ED1" s="25"/>
+      <c r="EE1" s="26"/>
+      <c r="EF1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="EG1" s="12"/>
-      <c r="EH1" s="12"/>
-      <c r="EI1" s="12"/>
-      <c r="EJ1" s="12"/>
-      <c r="EK1" s="12"/>
-      <c r="EL1" s="12"/>
-      <c r="EM1" s="12"/>
-      <c r="EN1" s="12"/>
-      <c r="EO1" s="12"/>
-      <c r="EP1" s="12"/>
-      <c r="EQ1" s="12"/>
-      <c r="ER1" s="12"/>
-      <c r="ES1" s="12"/>
-      <c r="ET1" s="12"/>
-      <c r="EU1" s="12"/>
-      <c r="EV1" s="12"/>
-      <c r="EW1" s="12"/>
-      <c r="EX1" s="12"/>
-      <c r="EY1" s="12"/>
-      <c r="EZ1" s="12"/>
-      <c r="FA1" s="12"/>
-      <c r="FB1" s="12"/>
-      <c r="FC1" s="12"/>
-      <c r="FD1" s="12"/>
-      <c r="FE1" s="12"/>
-      <c r="FF1" s="12"/>
-      <c r="FG1" s="12"/>
-      <c r="FH1" s="13"/>
+      <c r="EG1" s="25"/>
+      <c r="EH1" s="25"/>
+      <c r="EI1" s="25"/>
+      <c r="EJ1" s="25"/>
+      <c r="EK1" s="25"/>
+      <c r="EL1" s="25"/>
+      <c r="EM1" s="25"/>
+      <c r="EN1" s="25"/>
+      <c r="EO1" s="25"/>
+      <c r="EP1" s="25"/>
+      <c r="EQ1" s="25"/>
+      <c r="ER1" s="25"/>
+      <c r="ES1" s="25"/>
+      <c r="ET1" s="25"/>
+      <c r="EU1" s="25"/>
+      <c r="EV1" s="25"/>
+      <c r="EW1" s="25"/>
+      <c r="EX1" s="25"/>
+      <c r="EY1" s="25"/>
+      <c r="EZ1" s="25"/>
+      <c r="FA1" s="25"/>
+      <c r="FB1" s="25"/>
+      <c r="FC1" s="25"/>
+      <c r="FD1" s="25"/>
+      <c r="FE1" s="25"/>
+      <c r="FF1" s="25"/>
+      <c r="FG1" s="25"/>
+      <c r="FH1" s="26"/>
     </row>
     <row r="2" spans="1:241" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="8" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="8" t="s">
+      <c r="K2" s="23"/>
+      <c r="L2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="N2" s="8" t="s">
+      <c r="M2" s="23"/>
+      <c r="N2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="8" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="10"/>
-      <c r="W2" s="10"/>
-      <c r="X2" s="9"/>
-      <c r="Y2" s="8" t="s">
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="10"/>
-      <c r="AA2" s="10"/>
-      <c r="AB2" s="10"/>
-      <c r="AC2" s="10"/>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="9"/>
+      <c r="Z2" s="22"/>
+      <c r="AA2" s="22"/>
+      <c r="AB2" s="22"/>
+      <c r="AC2" s="22"/>
+      <c r="AD2" s="22"/>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="22"/>
+      <c r="AH2" s="23"/>
       <c r="AI2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AJ2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="9"/>
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="23"/>
       <c r="AP2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="AQ2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AR2" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="AS2" s="7"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="8" t="s">
+      <c r="AS2" s="19"/>
+      <c r="AT2" s="19"/>
+      <c r="AU2" s="19"/>
+      <c r="AV2" s="19"/>
+      <c r="AW2" s="19"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="AZ2" s="10"/>
-      <c r="BA2" s="10"/>
-      <c r="BB2" s="10"/>
-      <c r="BC2" s="10"/>
-      <c r="BD2" s="10"/>
-      <c r="BE2" s="10"/>
-      <c r="BF2" s="10"/>
-      <c r="BG2" s="9"/>
-      <c r="BH2" s="8" t="s">
+      <c r="AZ2" s="22"/>
+      <c r="BA2" s="22"/>
+      <c r="BB2" s="22"/>
+      <c r="BC2" s="22"/>
+      <c r="BD2" s="22"/>
+      <c r="BE2" s="22"/>
+      <c r="BF2" s="22"/>
+      <c r="BG2" s="23"/>
+      <c r="BH2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="BI2" s="10"/>
-      <c r="BJ2" s="10"/>
-      <c r="BK2" s="10"/>
-      <c r="BL2" s="10"/>
-      <c r="BM2" s="10"/>
-      <c r="BN2" s="10"/>
-      <c r="BO2" s="10"/>
-      <c r="BP2" s="10"/>
-      <c r="BQ2" s="9"/>
+      <c r="BI2" s="22"/>
+      <c r="BJ2" s="22"/>
+      <c r="BK2" s="22"/>
+      <c r="BL2" s="22"/>
+      <c r="BM2" s="22"/>
+      <c r="BN2" s="22"/>
+      <c r="BO2" s="22"/>
+      <c r="BP2" s="22"/>
+      <c r="BQ2" s="23"/>
       <c r="BR2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BS2" s="8" t="s">
+      <c r="BS2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="BT2" s="10"/>
-      <c r="BU2" s="10"/>
-      <c r="BV2" s="10"/>
-      <c r="BW2" s="10"/>
-      <c r="BX2" s="9"/>
+      <c r="BT2" s="22"/>
+      <c r="BU2" s="22"/>
+      <c r="BV2" s="22"/>
+      <c r="BW2" s="22"/>
+      <c r="BX2" s="23"/>
       <c r="BY2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="BZ2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="CA2" s="8" t="s">
+      <c r="CA2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="CB2" s="10"/>
-      <c r="CC2" s="10"/>
-      <c r="CD2" s="10"/>
-      <c r="CE2" s="10"/>
-      <c r="CF2" s="10"/>
-      <c r="CG2" s="10"/>
-      <c r="CH2" s="10"/>
-      <c r="CI2" s="9"/>
-      <c r="CJ2" s="8" t="s">
+      <c r="CB2" s="22"/>
+      <c r="CC2" s="22"/>
+      <c r="CD2" s="22"/>
+      <c r="CE2" s="22"/>
+      <c r="CF2" s="22"/>
+      <c r="CG2" s="22"/>
+      <c r="CH2" s="22"/>
+      <c r="CI2" s="23"/>
+      <c r="CJ2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="CK2" s="10"/>
-      <c r="CL2" s="10"/>
-      <c r="CM2" s="10"/>
-      <c r="CN2" s="10"/>
-      <c r="CO2" s="10"/>
-      <c r="CP2" s="10"/>
-      <c r="CQ2" s="10"/>
-      <c r="CR2" s="10"/>
-      <c r="CS2" s="9"/>
+      <c r="CK2" s="22"/>
+      <c r="CL2" s="22"/>
+      <c r="CM2" s="22"/>
+      <c r="CN2" s="22"/>
+      <c r="CO2" s="22"/>
+      <c r="CP2" s="22"/>
+      <c r="CQ2" s="22"/>
+      <c r="CR2" s="22"/>
+      <c r="CS2" s="23"/>
       <c r="CT2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="CU2" s="8" t="s">
+      <c r="CU2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="CV2" s="10"/>
-      <c r="CW2" s="10"/>
-      <c r="CX2" s="10"/>
-      <c r="CY2" s="10"/>
-      <c r="CZ2" s="9"/>
+      <c r="CV2" s="22"/>
+      <c r="CW2" s="22"/>
+      <c r="CX2" s="22"/>
+      <c r="CY2" s="22"/>
+      <c r="CZ2" s="23"/>
       <c r="DA2" s="2" t="s">
         <v>66</v>
       </c>
       <c r="DB2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="DC2" s="8" t="s">
+      <c r="DC2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="DD2" s="10"/>
-      <c r="DE2" s="10"/>
-      <c r="DF2" s="10"/>
-      <c r="DG2" s="10"/>
-      <c r="DH2" s="10"/>
-      <c r="DI2" s="10"/>
-      <c r="DJ2" s="10"/>
-      <c r="DK2" s="9"/>
-      <c r="DL2" s="8" t="s">
+      <c r="DD2" s="22"/>
+      <c r="DE2" s="22"/>
+      <c r="DF2" s="22"/>
+      <c r="DG2" s="22"/>
+      <c r="DH2" s="22"/>
+      <c r="DI2" s="22"/>
+      <c r="DJ2" s="22"/>
+      <c r="DK2" s="23"/>
+      <c r="DL2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="DM2" s="10"/>
-      <c r="DN2" s="10"/>
-      <c r="DO2" s="10"/>
-      <c r="DP2" s="10"/>
-      <c r="DQ2" s="10"/>
-      <c r="DR2" s="10"/>
-      <c r="DS2" s="10"/>
-      <c r="DT2" s="10"/>
-      <c r="DU2" s="9"/>
+      <c r="DM2" s="22"/>
+      <c r="DN2" s="22"/>
+      <c r="DO2" s="22"/>
+      <c r="DP2" s="22"/>
+      <c r="DQ2" s="22"/>
+      <c r="DR2" s="22"/>
+      <c r="DS2" s="22"/>
+      <c r="DT2" s="22"/>
+      <c r="DU2" s="23"/>
       <c r="DV2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="DW2" s="8" t="s">
+      <c r="DW2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="DX2" s="10"/>
-      <c r="DY2" s="10"/>
-      <c r="DZ2" s="10"/>
-      <c r="EA2" s="10"/>
-      <c r="EB2" s="9"/>
+      <c r="DX2" s="22"/>
+      <c r="DY2" s="22"/>
+      <c r="DZ2" s="22"/>
+      <c r="EA2" s="22"/>
+      <c r="EB2" s="23"/>
       <c r="EC2" s="2" t="s">
         <v>66</v>
       </c>
@@ -6780,40 +6780,40 @@
       <c r="EE2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="EF2" s="8" t="s">
+      <c r="EF2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="EG2" s="10"/>
-      <c r="EH2" s="10"/>
-      <c r="EI2" s="10"/>
-      <c r="EJ2" s="10"/>
-      <c r="EK2" s="10"/>
-      <c r="EL2" s="10"/>
-      <c r="EM2" s="10"/>
-      <c r="EN2" s="9"/>
-      <c r="EO2" s="8" t="s">
+      <c r="EG2" s="22"/>
+      <c r="EH2" s="22"/>
+      <c r="EI2" s="22"/>
+      <c r="EJ2" s="22"/>
+      <c r="EK2" s="22"/>
+      <c r="EL2" s="22"/>
+      <c r="EM2" s="22"/>
+      <c r="EN2" s="23"/>
+      <c r="EO2" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="EP2" s="10"/>
-      <c r="EQ2" s="10"/>
-      <c r="ER2" s="10"/>
-      <c r="ES2" s="10"/>
-      <c r="ET2" s="10"/>
-      <c r="EU2" s="10"/>
-      <c r="EV2" s="10"/>
-      <c r="EW2" s="10"/>
-      <c r="EX2" s="9"/>
+      <c r="EP2" s="22"/>
+      <c r="EQ2" s="22"/>
+      <c r="ER2" s="22"/>
+      <c r="ES2" s="22"/>
+      <c r="ET2" s="22"/>
+      <c r="EU2" s="22"/>
+      <c r="EV2" s="22"/>
+      <c r="EW2" s="22"/>
+      <c r="EX2" s="23"/>
       <c r="EY2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="EZ2" s="8" t="s">
+      <c r="EZ2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="FA2" s="10"/>
-      <c r="FB2" s="10"/>
-      <c r="FC2" s="10"/>
-      <c r="FD2" s="10"/>
-      <c r="FE2" s="9"/>
+      <c r="FA2" s="22"/>
+      <c r="FB2" s="22"/>
+      <c r="FC2" s="22"/>
+      <c r="FD2" s="22"/>
+      <c r="FE2" s="23"/>
       <c r="FF2" s="2" t="s">
         <v>66</v>
       </c>
@@ -6823,22 +6823,22 @@
       <c r="FH2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="FI2" s="4" t="s">
+      <c r="FI2" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="FJ2" s="19"/>
+      <c r="FK2" s="19"/>
+      <c r="FL2" s="20"/>
+      <c r="FM2" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="FN2" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="FJ2" s="7"/>
-      <c r="FK2" s="7"/>
-      <c r="FL2" s="7"/>
-      <c r="FM2" s="5"/>
-      <c r="FN2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="FO2" s="7"/>
-      <c r="FP2" s="7"/>
-      <c r="FQ2" s="5"/>
-      <c r="FR2" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="FO2" s="19"/>
+      <c r="FP2" s="19"/>
+      <c r="FQ2" s="19"/>
+      <c r="FR2" s="20"/>
     </row>
     <row r="3" spans="1:241" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
@@ -6865,7 +6865,7 @@
       <c r="H3" s="3">
         <v>7</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="10">
         <v>8</v>
       </c>
       <c r="J3" s="3">
@@ -6901,7 +6901,7 @@
       <c r="T3" s="3">
         <v>10</v>
       </c>
-      <c r="U3" s="19">
+      <c r="U3" s="10">
         <v>12</v>
       </c>
       <c r="V3" s="3">
@@ -6976,7 +6976,7 @@
       <c r="AS3" s="3">
         <v>6</v>
       </c>
-      <c r="AT3" s="19">
+      <c r="AT3" s="10">
         <v>7</v>
       </c>
       <c r="AU3" s="3">
@@ -7174,7 +7174,7 @@
       <c r="DG3" s="3">
         <v>10</v>
       </c>
-      <c r="DH3" s="19">
+      <c r="DH3" s="10">
         <v>12</v>
       </c>
       <c r="DI3" s="3">
@@ -7261,7 +7261,7 @@
       <c r="EJ3" s="3">
         <v>10</v>
       </c>
-      <c r="EK3" s="19">
+      <c r="EK3" s="10">
         <v>12</v>
       </c>
       <c r="EL3" s="3">
@@ -7333,35 +7333,35 @@
       <c r="FH3" s="3">
         <v>4</v>
       </c>
-      <c r="FI3" s="19">
+      <c r="FI3" s="3">
+        <v>3</v>
+      </c>
+      <c r="FJ3" s="3">
+        <v>5</v>
+      </c>
+      <c r="FK3" s="3">
+        <v>6</v>
+      </c>
+      <c r="FL3" s="3">
+        <v>7</v>
+      </c>
+      <c r="FM3" s="3">
+        <v>3</v>
+      </c>
+      <c r="FN3" s="10">
         <v>2</v>
       </c>
-      <c r="FJ3" s="3">
+      <c r="FO3" s="3">
         <v>4</v>
       </c>
-      <c r="FK3" s="3">
+      <c r="FP3" s="3">
         <v>5</v>
       </c>
-      <c r="FL3" s="3">
+      <c r="FQ3" s="3">
         <v>6</v>
       </c>
-      <c r="FM3" s="3">
+      <c r="FR3" s="3">
         <v>7</v>
-      </c>
-      <c r="FN3" s="3">
-        <v>3</v>
-      </c>
-      <c r="FO3" s="3">
-        <v>5</v>
-      </c>
-      <c r="FP3" s="3">
-        <v>6</v>
-      </c>
-      <c r="FQ3" s="3">
-        <v>7</v>
-      </c>
-      <c r="FR3" s="3">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:241" x14ac:dyDescent="0.2">
@@ -7371,10 +7371,10 @@
       <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -7389,7 +7389,7 @@
       <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="J4" s="2" t="s">
@@ -7398,22 +7398,22 @@
       <c r="K4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -7425,7 +7425,7 @@
       <c r="T4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="U4" s="19" t="s">
+      <c r="U4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="V4" s="2" t="s">
@@ -7437,7 +7437,7 @@
       <c r="X4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="Y4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="Z4" s="2" t="s">
@@ -7449,7 +7449,7 @@
       <c r="AB4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AC4" s="6" t="s">
+      <c r="AC4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="AD4" s="2" t="s">
@@ -7467,7 +7467,7 @@
       <c r="AH4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AI4" s="6" t="s">
+      <c r="AI4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="AJ4" s="2" t="s">
@@ -7488,19 +7488,19 @@
       <c r="AO4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AP4" s="6" t="s">
+      <c r="AP4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AQ4" s="6" t="s">
+      <c r="AQ4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AR4" s="6" t="s">
+      <c r="AR4" s="4" t="s">
         <v>71</v>
       </c>
       <c r="AS4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AT4" s="19" t="s">
+      <c r="AT4" s="10" t="s">
         <v>73</v>
       </c>
       <c r="AU4" s="2" t="s">
@@ -7515,10 +7515,10 @@
       <c r="AX4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AY4" s="6" t="s">
+      <c r="AY4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AZ4" s="6" t="s">
+      <c r="AZ4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="BA4" s="2" t="s">
@@ -7542,7 +7542,7 @@
       <c r="BG4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="BH4" s="6" t="s">
+      <c r="BH4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="BI4" s="2" t="s">
@@ -7554,7 +7554,7 @@
       <c r="BK4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="BL4" s="6" t="s">
+      <c r="BL4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="BM4" s="2" t="s">
@@ -7572,7 +7572,7 @@
       <c r="BQ4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BR4" s="6" t="s">
+      <c r="BR4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="BS4" s="2" t="s">
@@ -7593,16 +7593,16 @@
       <c r="BX4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="BY4" s="6" t="s">
+      <c r="BY4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BZ4" s="6" t="s">
+      <c r="BZ4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="CA4" s="6" t="s">
+      <c r="CA4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="CB4" s="6" t="s">
+      <c r="CB4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="CC4" s="2" t="s">
@@ -7626,7 +7626,7 @@
       <c r="CI4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="CJ4" s="6" t="s">
+      <c r="CJ4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="CK4" s="2" t="s">
@@ -7638,7 +7638,7 @@
       <c r="CM4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="CN4" s="6" t="s">
+      <c r="CN4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="CO4" s="2" t="s">
@@ -7656,7 +7656,7 @@
       <c r="CS4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="CT4" s="6" t="s">
+      <c r="CT4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="CU4" s="2" t="s">
@@ -7677,16 +7677,16 @@
       <c r="CZ4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="DA4" s="6" t="s">
+      <c r="DA4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="DB4" s="6" t="s">
+      <c r="DB4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="DC4" s="6" t="s">
+      <c r="DC4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="DD4" s="6" t="s">
+      <c r="DD4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="DE4" s="2" t="s">
@@ -7698,7 +7698,7 @@
       <c r="DG4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="DH4" s="19" t="s">
+      <c r="DH4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="DI4" s="2" t="s">
@@ -7710,7 +7710,7 @@
       <c r="DK4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="DL4" s="6" t="s">
+      <c r="DL4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="DM4" s="2" t="s">
@@ -7722,7 +7722,7 @@
       <c r="DO4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="DP4" s="6" t="s">
+      <c r="DP4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="DQ4" s="2" t="s">
@@ -7740,7 +7740,7 @@
       <c r="DU4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="DV4" s="6" t="s">
+      <c r="DV4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="DW4" s="2" t="s">
@@ -7761,19 +7761,19 @@
       <c r="EB4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="EC4" s="6" t="s">
+      <c r="EC4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="ED4" s="6" t="s">
+      <c r="ED4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="EE4" s="6" t="s">
+      <c r="EE4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="EF4" s="6" t="s">
+      <c r="EF4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="EG4" s="6" t="s">
+      <c r="EG4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="EH4" s="2" t="s">
@@ -7785,7 +7785,7 @@
       <c r="EJ4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="EK4" s="19" t="s">
+      <c r="EK4" s="10" t="s">
         <v>42</v>
       </c>
       <c r="EL4" s="2" t="s">
@@ -7797,7 +7797,7 @@
       <c r="EN4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="EO4" s="6" t="s">
+      <c r="EO4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="EP4" s="2" t="s">
@@ -7809,7 +7809,7 @@
       <c r="ER4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="ES4" s="6" t="s">
+      <c r="ES4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="ET4" s="2" t="s">
@@ -7827,7 +7827,7 @@
       <c r="EX4" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="EY4" s="6" t="s">
+      <c r="EY4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="EZ4" s="2" t="s">
@@ -7848,51 +7848,51 @@
       <c r="FE4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="FF4" s="6" t="s">
+      <c r="FF4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="FG4" s="6" t="s">
+      <c r="FG4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="FH4" s="6" t="s">
+      <c r="FH4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="FI4" s="14" t="s">
+      <c r="FI4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="FJ4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="FK4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="FL4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="FM4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="FN4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="FJ4" s="2" t="s">
+      <c r="FO4" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="FK4" s="2" t="s">
+      <c r="FP4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="FL4" s="2" t="s">
+      <c r="FQ4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="FM4" s="2" t="s">
+      <c r="FR4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="FN4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="FO4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="FP4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="FQ4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="FR4" s="6" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="5" spans="1:241" x14ac:dyDescent="0.2">
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="6" t="s">
         <v>1746</v>
       </c>
       <c r="P5" t="s">
@@ -7904,10 +7904,10 @@
       <c r="S5" t="s">
         <v>128</v>
       </c>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="U5" s="18" t="s">
+      <c r="U5" s="9" t="s">
         <v>1731</v>
       </c>
       <c r="V5" t="s">
@@ -7919,16 +7919,16 @@
       <c r="Z5" t="s">
         <v>1734</v>
       </c>
-      <c r="AA5" s="23" t="s">
+      <c r="AA5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AC5" s="24" t="s">
+      <c r="AC5" s="15" t="s">
         <v>7</v>
       </c>
       <c r="AE5" t="s">
         <v>351</v>
       </c>
-      <c r="AH5" s="26" t="s">
+      <c r="AH5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="AI5" t="s">
@@ -7943,20 +7943,20 @@
       <c r="AS5" s="1">
         <v>376214792611009</v>
       </c>
-      <c r="AT5" s="15" t="s">
+      <c r="AT5" s="6" t="s">
         <v>1737</v>
       </c>
-      <c r="AU5" s="20" t="s">
+      <c r="AU5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="FI5" s="15" t="s">
+      <c r="FI5" t="s">
+        <v>1709</v>
+      </c>
+      <c r="FM5" t="s">
+        <v>1723</v>
+      </c>
+      <c r="FN5" s="6" t="s">
         <v>1745</v>
-      </c>
-      <c r="FN5" t="s">
-        <v>1709</v>
-      </c>
-      <c r="FR5" t="s">
-        <v>1723</v>
       </c>
       <c r="FS5" t="s">
         <v>96</v>
@@ -8161,25 +8161,25 @@
       </c>
     </row>
     <row r="6" spans="1:241" x14ac:dyDescent="0.2">
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="6" t="s">
         <v>1746</v>
       </c>
       <c r="P6" t="s">
         <v>1729</v>
       </c>
-      <c r="Q6" s="20" t="s">
+      <c r="Q6" s="11" t="s">
         <v>1730</v>
       </c>
       <c r="S6" t="s">
         <v>128</v>
       </c>
-      <c r="T6" s="22" t="s">
+      <c r="T6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="U6" s="18" t="s">
+      <c r="U6" s="9" t="s">
         <v>1732</v>
       </c>
       <c r="V6" t="s">
@@ -8194,16 +8194,16 @@
       <c r="AA6" t="s">
         <v>6</v>
       </c>
-      <c r="AC6" s="16">
+      <c r="AC6" s="7">
         <v>510773</v>
       </c>
       <c r="AE6" t="s">
         <v>351</v>
       </c>
-      <c r="AF6" s="25" t="s">
+      <c r="AF6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AH6" s="26" t="s">
+      <c r="AH6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="AI6" t="s">
@@ -8218,16 +8218,16 @@
       <c r="AS6" s="1">
         <v>376211650141004</v>
       </c>
-      <c r="AT6" s="15" t="s">
+      <c r="AT6" s="6" t="s">
         <v>1738</v>
       </c>
-      <c r="AU6" s="20" t="s">
+      <c r="AU6" s="11" t="s">
         <v>14</v>
       </c>
       <c r="DC6" t="s">
         <v>1739</v>
       </c>
-      <c r="DD6" s="20" t="s">
+      <c r="DD6" s="11" t="s">
         <v>1740</v>
       </c>
       <c r="DF6" t="s">
@@ -8236,7 +8236,7 @@
       <c r="DG6" t="s">
         <v>11</v>
       </c>
-      <c r="DH6" s="15" t="s">
+      <c r="DH6" s="6" t="s">
         <v>1741</v>
       </c>
       <c r="DI6" t="s">
@@ -8251,16 +8251,16 @@
       <c r="DN6" t="s">
         <v>6</v>
       </c>
-      <c r="DP6" s="16">
+      <c r="DP6" s="7">
         <v>510773</v>
       </c>
       <c r="DR6" t="s">
         <v>351</v>
       </c>
-      <c r="DS6" s="26" t="s">
+      <c r="DS6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="DU6" s="26" t="s">
+      <c r="DU6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="DV6" t="s">
@@ -8272,10 +8272,10 @@
       <c r="EE6" t="s">
         <v>1700</v>
       </c>
-      <c r="EF6" s="20" t="s">
+      <c r="EF6" s="11" t="s">
         <v>1742</v>
       </c>
-      <c r="EG6" s="20" t="s">
+      <c r="EG6" s="11" t="s">
         <v>1743</v>
       </c>
       <c r="EI6" t="s">
@@ -8284,7 +8284,7 @@
       <c r="EJ6" t="s">
         <v>12</v>
       </c>
-      <c r="EK6" s="15" t="s">
+      <c r="EK6" s="6" t="s">
         <v>1744</v>
       </c>
       <c r="EL6" t="s">
@@ -8299,16 +8299,16 @@
       <c r="EQ6" t="s">
         <v>6</v>
       </c>
-      <c r="ES6" s="16">
+      <c r="ES6" s="7">
         <v>510773</v>
       </c>
       <c r="EU6" t="s">
         <v>351</v>
       </c>
-      <c r="EV6" s="26" t="s">
+      <c r="EV6" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="EX6" s="26" t="s">
+      <c r="EX6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="EY6" t="s">
@@ -8320,14 +8320,14 @@
       <c r="FH6" t="s">
         <v>1697</v>
       </c>
-      <c r="FI6" s="15" t="s">
+      <c r="FI6" t="s">
+        <v>1707</v>
+      </c>
+      <c r="FM6" t="s">
+        <v>1719</v>
+      </c>
+      <c r="FN6" s="6" t="s">
         <v>1745</v>
-      </c>
-      <c r="FN6" t="s">
-        <v>1707</v>
-      </c>
-      <c r="FR6" t="s">
-        <v>1719</v>
       </c>
       <c r="FS6" t="s">
         <v>97</v>
@@ -34182,8 +34182,26 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="FI2:FM2"/>
-    <mergeCell ref="FN2:FQ2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="Y2:AH2"/>
+    <mergeCell ref="AJ2:AO2"/>
+    <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="P1:AX1"/>
+    <mergeCell ref="AY2:BG2"/>
+    <mergeCell ref="P2:X2"/>
+    <mergeCell ref="BS2:BX2"/>
+    <mergeCell ref="AY1:BZ1"/>
+    <mergeCell ref="CA2:CI2"/>
+    <mergeCell ref="CJ2:CS2"/>
+    <mergeCell ref="CU2:CZ2"/>
+    <mergeCell ref="CA1:DB1"/>
+    <mergeCell ref="BH2:BQ2"/>
+    <mergeCell ref="FN2:FR2"/>
+    <mergeCell ref="FI2:FL2"/>
     <mergeCell ref="EZ2:FE2"/>
     <mergeCell ref="EF1:FH1"/>
     <mergeCell ref="DC2:DK2"/>
@@ -34192,24 +34210,6 @@
     <mergeCell ref="DC1:EE1"/>
     <mergeCell ref="EF2:EN2"/>
     <mergeCell ref="EO2:EX2"/>
-    <mergeCell ref="BS2:BX2"/>
-    <mergeCell ref="AY1:BZ1"/>
-    <mergeCell ref="CA2:CI2"/>
-    <mergeCell ref="CJ2:CS2"/>
-    <mergeCell ref="CU2:CZ2"/>
-    <mergeCell ref="CA1:DB1"/>
-    <mergeCell ref="Y2:AH2"/>
-    <mergeCell ref="AJ2:AO2"/>
-    <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="P1:AX1"/>
-    <mergeCell ref="AY2:BG2"/>
-    <mergeCell ref="BH2:BQ2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P2:X2"/>
   </mergeCells>
   <dataValidations count="67">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="C5:C65536">
@@ -34401,16 +34401,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FH5:FH65536">
       <formula1>$IC$5:$IC$25</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FJ5:FJ65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FO5:FO65536">
       <formula1>$ID$5:$ID$9</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FN5:FN65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FI5:FI65536">
       <formula1>$IE$5:$IE$10</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FQ5:FQ65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FL5:FL65536">
       <formula1>$IF$5:$IF$12</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FR5:FR65536">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please choose from of the following" sqref="FM5:FM65536">
       <formula1>$IG$5:$IG$12</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>